<commit_message>
Simple data passing sample now working.
</commit_message>
<xml_diff>
--- a/basics/passing_simple_data.xlsx
+++ b/basics/passing_simple_data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE444D2-6E25-4589-930D-CF6BB6D2BFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C059AC-D064-48A4-B1F3-85C9A9C2C379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3909" windowWidth="29426" windowHeight="13148" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="1517" yWindow="3771" windowWidth="29426" windowHeight="13149" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Workbook location</t>
   </si>
@@ -91,6 +90,13 @@
   </si>
   <si>
     <t>Using Python type hints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This workbook shows how type hints affect the behaviour of functions registered with xlSlim.
+The Python module passing_simple_data.py has many simple functions that either return the type of the argument passed to the function, or return a simple data type.
+The first set of function calls in C6:D10 show how type hints affect the types passed from Excel to Python. Note how xlSlim guesses floats, strings and bools correctly, however integers and datetimes need type hints to be handled correctly.
+The second set of function calls in B13:C17 show that xlSlim can correctly deduce the types of objects returned from Python even if type hints are not used. Type hints are always preferred though.
+</t>
   </si>
 </sst>
 </file>
@@ -132,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +156,13 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -174,13 +185,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -191,11 +267,30 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,21 +602,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774E7E1C-D275-4DD4-9028-FA14541EA3B8}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.84375" customWidth="1"/>
-    <col min="3" max="3" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.3046875" customWidth="1"/>
+    <col min="2" max="2" width="14.3828125" customWidth="1"/>
+    <col min="3" max="3" width="18.69140625" customWidth="1"/>
+    <col min="4" max="4" width="23.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -531,7 +626,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -541,7 +636,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -551,15 +646,25 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -574,8 +679,16 @@
         <f t="array" ref="D6">_xll.echo_type_int(B6)</f>
         <v>&lt;class 'int'&gt;</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -591,8 +704,16 @@
         <f t="array" ref="D7">_xll.echo_type_float(B7)</f>
         <v>&lt;class 'float'&gt;</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -607,8 +728,16 @@
         <f t="array" ref="D8">_xll.echo_type_string(B8)</f>
         <v>&lt;class 'str'&gt;</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -623,14 +752,22 @@
         <f t="array" ref="D9">_xll.echo_type_bool(B9)</f>
         <v>&lt;class 'bool'&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6">
         <f ca="1">NOW()</f>
-        <v>44667.477696180555</v>
+        <v>44667.507952430555</v>
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xll.echo_type(B10)</f>
@@ -640,16 +777,42 @@
         <f t="array" aca="1" ref="D10" ca="1">_xll.echo_type_datetime(B10)</f>
         <v>&lt;class 'datetime.datetime'&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
@@ -661,8 +824,16 @@
         <f t="array" ref="C13">_xll.return_int()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -674,8 +845,16 @@
         <f t="array" ref="C14">_xll.return_float()</f>
         <v>3.1415926535897931</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>6</v>
       </c>
@@ -687,8 +866,16 @@
         <f t="array" ref="C15">_xll.return_string()</f>
         <v>Hello!</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -700,27 +887,71 @@
         <f t="array" ref="C16">_xll.return_bool()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="6" cm="1">
         <f t="array" ref="B17">_xll.return_datetime_no_type_hints()</f>
-        <v>44667.477685185186</v>
+        <v>44667.507951388892</v>
       </c>
       <c r="C17" s="6" cm="1">
         <f t="array" ref="C17">_xll.return_datetime()</f>
-        <v>44667.477685185186</v>
-      </c>
+        <v>44667.507951388892</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E5:L18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A28DAB99C48B469009752D21F8474A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3725108ba1e248dd961cbde49d36f75">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="58a034177a2e5a667d336d2ca3036430" ns3:_="">
     <xsd:import namespace="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
@@ -852,22 +1083,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C9D94B-68A3-4C5A-8543-29DBB1AA8066}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -883,28 +1123,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>